<commit_message>
Refactors logic into separate js file
</commit_message>
<xml_diff>
--- a/excel_files/balance2.xlsx
+++ b/excel_files/balance2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmuther/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DD31BD-B65B-184E-B5EF-543B577B724C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954CB9E7-6C53-9C4B-93F3-2D3A76D41CC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="900" windowWidth="27640" windowHeight="15800" xr2:uid="{F9D0B887-BBDE-3543-8C7D-69882DB4E8A8}"/>
   </bookViews>
@@ -397,7 +397,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>